<commit_message>
Fitted Theta_m to a polynomial function
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/Theta_m values.xlsx
+++ b/Wastewater_Effluent_Filtration/Theta_m values.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923FED1B-CC25-4CF4-BDC0-683804F05C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6B4352-865F-4B2B-8250-8DFA775004A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Theta vs pH" sheetId="1" r:id="rId1"/>
+    <sheet name="Theta" sheetId="1" r:id="rId1"/>
     <sheet name="NH4+ Permeability" sheetId="2" r:id="rId2"/>
+    <sheet name="NaCl Permeability" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateCount="300" iterateDelta="1E-25"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>BW30LE</t>
   </si>
@@ -71,6 +72,9 @@
   <si>
     <t>Dow Filmtec SW30HRLE</t>
   </si>
+  <si>
+    <t>W_NaCl</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,12 +113,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,9 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -170,12 +171,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -188,10 +183,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -305,7 +300,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Theta vs pH'!$D$2</c:f>
+              <c:f>Theta!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,8 +350,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="9.768873673399521E-2"/>
-                  <c:y val="0.36866230704212821"/>
+                  <c:x val="-5.8857305593399065E-3"/>
+                  <c:y val="-0.1210398265434212"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -378,18 +373,18 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
                       <a:t>y = -0.0486x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="30000"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
                       <a:t>2</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
                       <a:t> + 0.7373x - 2.6937</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -425,7 +420,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$C$3:$C$5</c:f>
+              <c:f>Theta!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -443,7 +438,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$D$3:$D$5</c:f>
+              <c:f>Theta!$D$3:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -654,6 +649,876 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Dow Filmtec XLE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NaCl Permeability'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_NaCl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1215659005191196"/>
+                  <c:y val="8.5010360547036878E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = -2E-08x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:t> + 3E-07x - 4E-07</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-IL" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$G$4:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.4799999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.96E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8999999999999998E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8F9-4324-AF84-F028D058E9A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1036938271"/>
+        <c:axId val="974340287"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1036938271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="974340287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="974340287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1036938271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Dow Filmtec SW30HRLE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NaCl Permeability'!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_NaCl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.20673600174978127"/>
+                  <c:y val="8.7546296296296303E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                        <a:latin typeface="+mn-lt"/>
+                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t>y = 1E-09x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000">
+                        <a:latin typeface="+mn-lt"/>
+                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                        <a:latin typeface="+mn-lt"/>
+                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t> - 1E-08x + 1E-07</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1">
+                      <a:latin typeface="+mn-lt"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$M$4:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$N$4:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.7399999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8799999999999994E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7299999999999997E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-819C-4199-BA1F-2134E507DD64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1547037407"/>
+        <c:axId val="1190479199"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1547037407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1190479199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1190479199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1547037407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -744,7 +1609,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Theta vs pH'!$K$2</c:f>
+              <c:f>Theta!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -787,14 +1652,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.3241525867492634E-2"/>
-                  <c:y val="0.26677569150010094"/>
+                  <c:x val="-0.23084352777702094"/>
+                  <c:y val="3.3548832711700512E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -816,17 +1682,18 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0"/>
-                      <a:t>y = 0.1455x - 0.8153</a:t>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = -0.031x</a:t>
                     </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" b="1" baseline="0"/>
-                    </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0"/>
-                      <a:t>R² = 0.9515</a:t>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" b="1"/>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> + 0.5433x - 2.0069</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -862,7 +1729,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$J$3:$J$5</c:f>
+              <c:f>Theta!$J$3:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -880,7 +1747,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$K$3:$K$5</c:f>
+              <c:f>Theta!$K$3:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1171,7 +2038,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Theta vs pH'!$Q$2</c:f>
+              <c:f>Theta!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1214,16 +2081,51 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.26677184084095745"/>
-                  <c:y val="0.12223152022315202"/>
+                  <c:x val="-9.7630368526814143E-2"/>
+                  <c:y val="8.6939890710382509E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = 0.0154x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> - 0.1067x + 0.2683</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1256,7 +2158,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$P$3:$P$5</c:f>
+              <c:f>Theta!$P$3:$P$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1274,7 +2176,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$Q$3:$Q$5</c:f>
+              <c:f>Theta!$Q$3:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1564,7 +2466,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Theta vs pH'!$G$23</c:f>
+              <c:f>Theta!$G$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1607,16 +2509,51 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.29605161854768153"/>
-                  <c:y val="0.18454421768707482"/>
+                  <c:x val="-0.23684317585301837"/>
+                  <c:y val="8.4728620152427464E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = -0.0323x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> + 0.6078x - 2.3605</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1649,7 +2586,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$F$24:$F$26</c:f>
+              <c:f>Theta!$F$24:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1667,7 +2604,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Theta vs pH'!$G$24:$G$26</c:f>
+              <c:f>Theta!$G$24:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3573,7 +4510,523 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dow Filmtec BW30LE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NaCl Permeability'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_NaCl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7510081776240668E-2"/>
+                  <c:y val="-0.4176197375328084"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = 3E-09x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> - 4E-08x + 4E-07</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NaCl Permeability'!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.8200000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5499999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5499999999999999E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CA1-4EFD-8589-525CC77698CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1197587743"/>
+        <c:axId val="1197718415"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1197587743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1197718415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1197718415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1197587743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3893,6 +5346,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4409,7 +5902,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4925,7 +6418,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5441,7 +6934,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5957,7 +7450,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6473,7 +7966,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6989,7 +8482,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7505,7 +8998,1555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8027,12 +11068,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
@@ -8061,14 +11102,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>546099</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -8097,16 +11138,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8133,16 +11174,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>422275</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>117475</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8319,6 +11360,119 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF86DD8F-003F-1D2A-F79A-976471AE64E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B735C0B7-2DE7-5D43-935C-E0556D8D823D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C214AE4F-CBAE-5046-9266-3F9AECCEACE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8618,25 +11772,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D8DF6C-B2F6-4A6F-8293-0BD351469548}">
   <dimension ref="C1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="P1" s="6" t="s">
+      <c r="K1" s="6"/>
+      <c r="P1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="7"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
@@ -8719,10 +11873,10 @@
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
@@ -8772,29 +11926,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2084F8-C00A-4FC4-9424-2C4DB9F35A7A}">
   <dimension ref="C2:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="J2" s="10" t="s">
+      <c r="D2" s="12"/>
+      <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="O2" s="12" t="s">
+      <c r="K2" s="10"/>
+      <c r="O2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="S2" s="10" t="s">
+      <c r="P2" s="14"/>
+      <c r="S2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="11"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
@@ -8910,4 +12064,149 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F470B7BE-6E9D-48F7-9952-EB31E3934660}">
+  <dimension ref="B2:S6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="G22:H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="G2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="M2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="R2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="10"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.8200000000000001E-7</v>
+      </c>
+      <c r="G4">
+        <v>4.5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3.4799999999999999E-7</v>
+      </c>
+      <c r="M4">
+        <v>4.5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>6.7399999999999995E-8</v>
+      </c>
+      <c r="R4">
+        <v>4.5</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3.41E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.5499999999999999E-7</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.96E-7</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5" s="1">
+        <v>6.8799999999999994E-8</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
+      <c r="S5" s="1">
+        <v>3.1699999999999999E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>8.5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.5499999999999999E-7</v>
+      </c>
+      <c r="G6">
+        <v>8.5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.8999999999999998E-7</v>
+      </c>
+      <c r="M6">
+        <v>8.5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>7.7299999999999997E-8</v>
+      </c>
+      <c r="R6">
+        <v>8.5</v>
+      </c>
+      <c r="S6" s="1">
+        <v>2.5499999999999999E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fitted Salt permeability and Water Permeability to Polynomial functions.
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/Theta_m values.xlsx
+++ b/Wastewater_Effluent_Filtration/Theta_m values.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6B4352-865F-4B2B-8250-8DFA775004A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AFCA61-EFF3-425A-8B2E-F64ECD6DC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
   </bookViews>
   <sheets>
     <sheet name="Theta" sheetId="1" r:id="rId1"/>
     <sheet name="NH4+ Permeability" sheetId="2" r:id="rId2"/>
     <sheet name="NaCl Permeability" sheetId="3" r:id="rId3"/>
+    <sheet name="Water Permeability" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateCount="300" iterateDelta="1E-25"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
   <si>
     <t>BW30LE</t>
   </si>
@@ -75,11 +76,20 @@
   <si>
     <t>W_NaCl</t>
   </si>
+  <si>
+    <t>W_H2O</t>
+  </si>
+  <si>
+    <t>W_H2O (m/s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,12 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -165,6 +176,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -175,12 +192,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -779,8 +790,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.1215659005191196"/>
-                  <c:y val="8.5010360547036878E-3"/>
+                  <c:x val="-8.9447327371371399E-2"/>
+                  <c:y val="-1.2070735633183973E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -802,18 +813,18 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
                       <a:t>y = -2E-08x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="30000"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
                       <a:t>2</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
                       <a:t> + 3E-07x - 4E-07</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-IL" sz="1200" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1464,6 +1475,1728 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1547037407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Dow Filmtec BW30LE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33993366500829186"/>
+          <c:y val="3.3432842107480008E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Water Permeability'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_H2O (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.295306006213475E-2"/>
+                  <c:y val="0.11092979482937339"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = 5E-08x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> - 7E-07x + 3E-06</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$B$5:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3888888888888883E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9444444444444448E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DB0-4DDF-AC54-013DAB817AA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1193733951"/>
+        <c:axId val="1332518623"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1193733951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332518623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1332518623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1193733951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Dow Filmtec XLE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Water Permeability'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_H2O (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0517613223335423E-3"/>
+                  <c:y val="-0.58802988546152946"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = -5E-09x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> + 6E-08x + 8E-07</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$H$5:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$J$5:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.5555555555555561E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4527777777777777E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0611111111111109E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C1F-4EC7-BCCC-5766278473D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1421570944"/>
+        <c:axId val="1412225424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1421570944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1412225424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1412225424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1421570944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Dow Filmtec SW30HRLE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Water Permeability'!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_H2O (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.8282287207083967E-2"/>
+                  <c:y val="5.5512173461640842E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = 9E-09x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t> - 1E-07x + 7E-07</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$N$5:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$P$5:$P$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.6166666666666666E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2777777777777776E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6416666666666664E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9D44-4910-AA46-51EE35C7D90A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1332272831"/>
+        <c:axId val="1412221952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1332272831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1412221952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1412221952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332272831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>SUEZ AG</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Water Permeability'!$W$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W_H2O (m/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.23755391894623548"/>
+                  <c:y val="0.29494920165902344"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:t>y = 4E-08x + 4E-07</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-IL" sz="1200" b="1" baseline="0"/>
+                      <a:t>R² = 0.9593</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-IL" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-IL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$U$5:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Water Permeability'!$W$5:$W$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.5444444444444444E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2777777777777774E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1805555555555555E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F4F-4E02-BE88-BDEDFB5EC40B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1421560384"/>
+        <c:axId val="1412224928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1421560384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1412224928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1412224928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1421560384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4640,15 +6373,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.7510081776240668E-2"/>
-                  <c:y val="-0.4176197375328084"/>
+                  <c:x val="-9.4955481780200773E-3"/>
+                  <c:y val="-0.46561973753280839"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -4671,15 +6403,7 @@
                     </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
-                      <a:t>y = 3E-09x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
-                      <a:t> - 4E-08x + 4E-07</a:t>
+                      <a:t>y = -1E-08x + 3E-07</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US" sz="1200" b="1"/>
                   </a:p>
@@ -4727,25 +6451,22 @@
                 <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'NaCl Permeability'!$C$4:$C$6</c:f>
+              <c:f>'NaCl Permeability'!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.8200000000000001E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.5499999999999999E-7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2.5499999999999999E-7</c:v>
                 </c:pt>
               </c:numCache>
@@ -5027,6 +6748,166 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6419,6 +8300,2070 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11473,6 +15418,155 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>125412</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2454F08D-9D87-439A-57CF-DCF6042EC92A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>49213</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>153987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D25F8D7-29CF-6C5E-4987-E9355A7F0125}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8979468-BA8E-9788-FD20-8B40CA716D8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>144462</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84D6CD41-A12A-7926-8F8C-91C2C74CF140}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11772,25 +15866,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D8DF6C-B2F6-4A6F-8293-0BD351469548}">
   <dimension ref="C1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="J1" s="5" t="s">
+      <c r="E1" s="5"/>
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="P1" s="11" t="s">
+      <c r="K1" s="7"/>
+      <c r="P1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="12"/>
+      <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
@@ -11873,10 +15967,10 @@
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="8"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
@@ -11933,22 +16027,22 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="3:20" x14ac:dyDescent="0.35">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="J2" s="9" t="s">
+      <c r="D2" s="9"/>
+      <c r="J2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="O2" s="13" t="s">
+      <c r="K2" s="13"/>
+      <c r="O2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="S2" s="9" t="s">
+      <c r="P2" s="15"/>
+      <c r="S2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="10"/>
+      <c r="T2" s="13"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
@@ -12068,31 +16162,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F470B7BE-6E9D-48F7-9952-EB31E3934660}">
-  <dimension ref="B2:S6"/>
+  <dimension ref="B2:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="G22:H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="G2" s="9" t="s">
+      <c r="C2" s="13"/>
+      <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="M2" s="9" t="s">
+      <c r="H2" s="13"/>
+      <c r="M2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="R2" s="9" t="s">
+      <c r="N2" s="13"/>
+      <c r="R2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="10"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
@@ -12173,12 +16267,6 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <v>8.5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.5499999999999999E-7</v>
-      </c>
       <c r="G6">
         <v>8.5</v>
       </c>
@@ -12198,6 +16286,14 @@
         <v>2.5499999999999999E-7</v>
       </c>
     </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>8.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.5499999999999999E-7</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
@@ -12209,4 +16305,218 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2FC76E-EEA0-44C2-AC05-8BC5F5E9CBFB}">
+  <dimension ref="B3:W7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="H3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="N3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="U3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="13"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>3600000</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>4.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5/E4</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H5">
+        <v>4.5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.44</v>
+      </c>
+      <c r="J5">
+        <f>I5/E4</f>
+        <v>9.5555555555555561E-7</v>
+      </c>
+      <c r="N5">
+        <v>4.5</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1.302</v>
+      </c>
+      <c r="P5">
+        <f>O5/E4</f>
+        <v>3.6166666666666666E-7</v>
+      </c>
+      <c r="U5">
+        <v>4.5</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1.996</v>
+      </c>
+      <c r="W5">
+        <f>V5/E4</f>
+        <v>5.5444444444444444E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6/E4</f>
+        <v>6.3888888888888883E-7</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.403</v>
+      </c>
+      <c r="J6">
+        <f>I6/E4</f>
+        <v>9.4527777777777777E-7</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="P6">
+        <f>O6/E4</f>
+        <v>3.2777777777777776E-7</v>
+      </c>
+      <c r="U6">
+        <v>7</v>
+      </c>
+      <c r="V6" s="3">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="W6">
+        <f>V6/E4</f>
+        <v>6.2777777777777774E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>8.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7/E4</f>
+        <v>6.9444444444444448E-7</v>
+      </c>
+      <c r="H7">
+        <v>8.5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.262</v>
+      </c>
+      <c r="J7">
+        <f>I7/E4</f>
+        <v>9.0611111111111109E-7</v>
+      </c>
+      <c r="N7">
+        <v>8.5</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="P7">
+        <f>O7/E4</f>
+        <v>3.6416666666666664E-7</v>
+      </c>
+      <c r="U7">
+        <v>8.5</v>
+      </c>
+      <c r="V7" s="3">
+        <v>2.585</v>
+      </c>
+      <c r="W7">
+        <f>V7/E4</f>
+        <v>7.1805555555555555E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="U3:V3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated index notation for pH_b
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/Theta_m values.xlsx
+++ b/Wastewater_Effluent_Filtration/Theta_m values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AFCA61-EFF3-425A-8B2E-F64ECD6DC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F383FF4-9F28-4D5C-B39F-939BD020448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
   </bookViews>
   <sheets>
     <sheet name="Theta" sheetId="1" r:id="rId1"/>
@@ -16164,7 +16164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F470B7BE-6E9D-48F7-9952-EB31E3934660}">
   <dimension ref="B2:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -16311,8 +16311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2FC76E-EEA0-44C2-AC05-8BC5F5E9CBFB}">
   <dimension ref="B3:W7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added aerobic MBR file
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/Theta_m values.xlsx
+++ b/Wastewater_Effluent_Filtration/Theta_m values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F383FF4-9F28-4D5C-B39F-939BD020448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE330AB3-353E-42CF-B8E1-6792C511712C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
   </bookViews>
   <sheets>
     <sheet name="Theta" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="NaCl Permeability" sheetId="3" r:id="rId3"/>
     <sheet name="Water Permeability" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="300" iterateDelta="1E-25"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -16021,7 +16021,7 @@
   <dimension ref="C2:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16169,6 +16169,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
@@ -16312,7 +16315,7 @@
   <dimension ref="B3:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Aerobic MBR Interface file
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/Theta_m values.xlsx
+++ b/Wastewater_Effluent_Filtration/Theta_m values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6894419-4ED6-49AB-B660-37A4943E26C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2018C485-1FE3-4ADF-89A7-03C8F18BA800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
+    <workbookView xWindow="-28920" yWindow="960" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0EF10369-FB7A-474D-9972-95E7D59C006E}"/>
   </bookViews>
   <sheets>
     <sheet name="Theta" sheetId="1" r:id="rId1"/>
@@ -15854,7 +15854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D8DF6C-B2F6-4A6F-8293-0BD351469548}">
   <dimension ref="C1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -16012,7 +16012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2084F8-C00A-4FC4-9424-2C4DB9F35A7A}">
   <dimension ref="C2:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -16149,7 +16149,7 @@
   <dimension ref="B2:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16299,7 +16299,7 @@
   <dimension ref="B3:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>